<commit_message>
Added agent design outline/pseudocode to docs folder
</commit_message>
<xml_diff>
--- a/docs/8puzzleManualStateSpace.xlsx
+++ b/docs/8puzzleManualStateSpace.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgarrettsisk/Development/assignment02/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C642AA12-A934-EE40-839D-8F8DA0779238}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D738DDF8-CF95-C149-B757-A3BF403CE7F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="23860" xr2:uid="{CC52E3EC-35AE-504B-B117-24855AEA39E0}"/>
+    <workbookView xWindow="13400" yWindow="4960" windowWidth="40960" windowHeight="23860" xr2:uid="{CC52E3EC-35AE-504B-B117-24855AEA39E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -544,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EB0778-B27F-C14D-B0DD-C33D21530681}">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added additional information regarding outline for agent. Added prototype GUI into src folder.
</commit_message>
<xml_diff>
--- a/docs/8puzzleManualStateSpace.xlsx
+++ b/docs/8puzzleManualStateSpace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgarrettsisk/Development/assignment02/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D738DDF8-CF95-C149-B757-A3BF403CE7F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48628DF-C202-3245-A434-0A895DFD4217}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="4960" windowWidth="40960" windowHeight="23860" xr2:uid="{CC52E3EC-35AE-504B-B117-24855AEA39E0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{CC52E3EC-35AE-504B-B117-24855AEA39E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EB0778-B27F-C14D-B0DD-C33D21530681}">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>